<commit_message>
sample slsx file changes
</commit_message>
<xml_diff>
--- a/src/main/resources/static/assets/download-sample.xlsx
+++ b/src/main/resources/static/assets/download-sample.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
   <si>
     <t>Mobile Number</t>
   </si>
@@ -79,6 +79,12 @@
   </si>
   <si>
     <t>City Bank</t>
+  </si>
+  <si>
+    <t>123456789</t>
+  </si>
+  <si>
+    <t>987654321</t>
   </si>
 </sst>
 </file>
@@ -137,7 +143,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -158,6 +164,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -462,7 +471,7 @@
   <dimension ref="A1:I74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -532,8 +541,8 @@
       <c r="E3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="5">
-        <v>123456789</v>
+      <c r="F3" s="10" t="s">
+        <v>21</v>
       </c>
       <c r="G3" s="5" t="s">
         <v>12</v>
@@ -561,8 +570,8 @@
       <c r="E4" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="5">
-        <v>987654321</v>
+      <c r="F4" s="10" t="s">
+        <v>22</v>
       </c>
       <c r="G4" s="5" t="s">
         <v>19</v>

</xml_diff>